<commit_message>
se modifica E-R, y se agrega el doc APPMO-SP_ARP_v1.0.xlsx
</commit_message>
<xml_diff>
--- a/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.0.xlsx
+++ b/Entregables/V. Análisis de riesgo del proyecto de TI/APPMO-SP_ARP_v1.0.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="124">
   <si>
     <t>Probabilidad</t>
   </si>
@@ -314,15 +314,6 @@
     <t>Pérdida de información</t>
   </si>
   <si>
-    <t>Daño en el equipo de cómputo</t>
-  </si>
-  <si>
-    <t>Mala instalación eléctrica</t>
-  </si>
-  <si>
-    <t>Verificar la instalación electrica del local y utilizar no breaks</t>
-  </si>
-  <si>
     <t>Programador</t>
   </si>
   <si>
@@ -338,20 +329,126 @@
     <t>Retrazo en entregables del producto</t>
   </si>
   <si>
-    <t>Tiempos incongruentes y fechas mal planeadas.</t>
-  </si>
-  <si>
     <t>Revisar actividades con fechas y ajustarlos a tiempos del proyecto.</t>
   </si>
   <si>
-    <t>Las actvidades</t>
+    <t>Documentos de planeación e implementación del Software</t>
+  </si>
+  <si>
+    <t>Requerimientos ambiguos o incompletos</t>
+  </si>
+  <si>
+    <t>Cambios regulares y nuevos añadidos a los requerimientos</t>
+  </si>
+  <si>
+    <t>Mala comunicación con el cliente</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Diseño de interfaces incompletos</t>
+  </si>
+  <si>
+    <t>Incorrecta definición y estructura de los datos</t>
+  </si>
+  <si>
+    <t>Mal entendimiento de las
+relaciones y dependencias del producto</t>
+  </si>
+  <si>
+    <t>Diseñador</t>
+  </si>
+  <si>
+    <t>Analista</t>
+  </si>
+  <si>
+    <t>Diseño de interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acomplar los nuevos cambios o requetimientos a los existentes de forma clara y completa para cumplir la funcionalidad planeada </t>
+  </si>
+  <si>
+    <t>Desarrollo/Codificación</t>
+  </si>
+  <si>
+    <t>Falta de respaldo de información</t>
+  </si>
+  <si>
+    <t>Retrazo de avances con el software</t>
+  </si>
+  <si>
+    <t>Mala organización del equipo de trabajo</t>
+  </si>
+  <si>
+    <t>Tiempos incongruentes y fechas mal planeadas</t>
+  </si>
+  <si>
+    <t>Organización ineficiente</t>
+  </si>
+  <si>
+    <t>•Definir nomenclatura para cada archivo sujeto con un control de versión
+•Crear un repositorio en la nube para subir y bajar actualizaciónes</t>
+  </si>
+  <si>
+    <t>Todos los miembros del equipo de trabajo tienen acceso al repositorio creado</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
+  </si>
+  <si>
+    <t>Presentación de defectos en ambientes de producción</t>
+  </si>
+  <si>
+    <t>Retrazo en entregables del proyecto</t>
+  </si>
+  <si>
+    <t>Mala realización de pruebas</t>
+  </si>
+  <si>
+    <t>Pruebas ineficientes</t>
+  </si>
+  <si>
+    <t>•Realizar pruebas de cada modulo de la aplicación detalladamente
+•Darle seguimiento a cada falla encontrado
+•Volver a probar los módulos donde hubieron fallas</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Codificiación</t>
+  </si>
+  <si>
+    <t>Análista</t>
+  </si>
+  <si>
+    <t>Los nuevos cambios a los requisitos se acomplan a los ya dados antes.</t>
+  </si>
+  <si>
+    <t>Se crea un diagrama de las actividades y tiempos</t>
+  </si>
+  <si>
+    <t>La estructura es diferente a los diseños, al ser un software móvil, su propia naturaleza afecta a la codificación misma.</t>
+  </si>
+  <si>
+    <t>Incorrecta interpretación de las ventanas e interfaces</t>
+  </si>
+  <si>
+    <t>Rediseñar las interfaces con base  a las especificaciónes de requerimientos</t>
+  </si>
+  <si>
+    <t>Definir la arquitectura lógica y las relaciones correctas con base a los procesos de la empresa</t>
+  </si>
+  <si>
+    <t>Mal entendimiento de los requerimientos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -418,6 +515,11 @@
     <font>
       <b/>
       <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1117,7 +1219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1435,6 +1537,36 @@
     <xf numFmtId="14" fontId="7" fillId="18" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1462,6 +1594,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1471,49 +1648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1522,9 +1657,6 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1534,29 +1666,8 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1908,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1929,18 +2040,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="120"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
@@ -1967,18 +2078,18 @@
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
+      <c r="B4" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
       <c r="E4" s="13"/>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
       <c r="J4" s="13"/>
       <c r="K4" s="14"/>
     </row>
@@ -1999,10 +2110,10 @@
       <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="121"/>
+      <c r="I5" s="131"/>
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>
     </row>
@@ -2023,10 +2134,10 @@
       <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="121" t="s">
+      <c r="H6" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="121"/>
+      <c r="I6" s="131"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
     </row>
@@ -2047,10 +2158,10 @@
       <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="121" t="s">
+      <c r="H7" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="121"/>
+      <c r="I7" s="131"/>
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
     </row>
@@ -2071,10 +2182,10 @@
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="121" t="s">
+      <c r="H8" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="121"/>
+      <c r="I8" s="131"/>
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
     </row>
@@ -2095,10 +2206,10 @@
       <c r="G9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="122" t="s">
+      <c r="H9" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="122"/>
+      <c r="I9" s="132"/>
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
     </row>
@@ -2139,32 +2250,32 @@
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="124" t="s">
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="124"/>
+      <c r="I13" s="134"/>
       <c r="J13" s="8" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="117"/>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="117"/>
+      <c r="B14" s="127"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
@@ -2202,7 +2313,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="102">
         <v>1</v>
       </c>
@@ -2210,29 +2321,29 @@
         <v>80</v>
       </c>
       <c r="D16" s="104" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E16" s="105" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="F16" s="106" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="G16" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="150">
-        <v>2</v>
-      </c>
-      <c r="I16" s="150">
+      <c r="H16" s="119">
+        <v>3</v>
+      </c>
+      <c r="I16" s="119">
         <v>4</v>
       </c>
-      <c r="J16" s="151">
+      <c r="J16" s="120">
         <f t="shared" ref="J16:J30" si="0">H16*I16</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K16" s="112" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -2243,114 +2354,162 @@
         <v>80</v>
       </c>
       <c r="D17" s="90" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="E17" s="93" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F17" s="96" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G17" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="152">
+        <v>110</v>
+      </c>
+      <c r="H17" s="121">
         <v>3</v>
       </c>
-      <c r="I17" s="152">
+      <c r="I17" s="121">
         <v>4</v>
       </c>
-      <c r="J17" s="153">
+      <c r="J17" s="122">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="K17" s="108" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22">
         <v>3</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="154">
-        <v>0</v>
-      </c>
-      <c r="I18" s="154">
-        <v>0</v>
-      </c>
-      <c r="J18" s="155">
+      <c r="C18" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="100" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="123">
+        <v>3</v>
+      </c>
+      <c r="I18" s="123">
+        <v>4</v>
+      </c>
+      <c r="J18" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="109"/>
-    </row>
-    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="K18" s="109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22">
         <v>4</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="154">
-        <v>0</v>
-      </c>
-      <c r="I19" s="154">
-        <v>0</v>
-      </c>
-      <c r="J19" s="155">
+      <c r="C19" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="123">
+        <v>2</v>
+      </c>
+      <c r="I19" s="123">
+        <v>3</v>
+      </c>
+      <c r="J19" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="109"/>
-    </row>
-    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="K19" s="160" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22">
         <v>5</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="100"/>
-      <c r="H20" s="154">
-        <v>0</v>
-      </c>
-      <c r="I20" s="154">
-        <v>0</v>
-      </c>
-      <c r="J20" s="155">
+      <c r="C20" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="123">
+        <v>3</v>
+      </c>
+      <c r="I20" s="123">
+        <v>4</v>
+      </c>
+      <c r="J20" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="109"/>
-    </row>
-    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="K20" s="160" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22">
         <v>6</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="154">
-        <v>0</v>
-      </c>
-      <c r="I21" s="154">
-        <v>0</v>
-      </c>
-      <c r="J21" s="155">
+      <c r="C21" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="97" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="100" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="123">
+        <v>3</v>
+      </c>
+      <c r="I21" s="123">
+        <v>5</v>
+      </c>
+      <c r="J21" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="109"/>
+        <v>15</v>
+      </c>
+      <c r="K21" s="109" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22">
@@ -2361,13 +2520,13 @@
       <c r="E22" s="94"/>
       <c r="F22" s="97"/>
       <c r="G22" s="100"/>
-      <c r="H22" s="154">
-        <v>0</v>
-      </c>
-      <c r="I22" s="154">
-        <v>0</v>
-      </c>
-      <c r="J22" s="155">
+      <c r="H22" s="123">
+        <v>0</v>
+      </c>
+      <c r="I22" s="123">
+        <v>0</v>
+      </c>
+      <c r="J22" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2382,13 +2541,13 @@
       <c r="E23" s="94"/>
       <c r="F23" s="97"/>
       <c r="G23" s="100"/>
-      <c r="H23" s="154">
-        <v>0</v>
-      </c>
-      <c r="I23" s="154">
-        <v>0</v>
-      </c>
-      <c r="J23" s="155">
+      <c r="H23" s="123">
+        <v>0</v>
+      </c>
+      <c r="I23" s="123">
+        <v>0</v>
+      </c>
+      <c r="J23" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2403,13 +2562,13 @@
       <c r="E24" s="94"/>
       <c r="F24" s="97"/>
       <c r="G24" s="100"/>
-      <c r="H24" s="154">
-        <v>0</v>
-      </c>
-      <c r="I24" s="154">
-        <v>0</v>
-      </c>
-      <c r="J24" s="155">
+      <c r="H24" s="123">
+        <v>0</v>
+      </c>
+      <c r="I24" s="123">
+        <v>0</v>
+      </c>
+      <c r="J24" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2424,13 +2583,13 @@
       <c r="E25" s="94"/>
       <c r="F25" s="97"/>
       <c r="G25" s="100"/>
-      <c r="H25" s="154">
-        <v>0</v>
-      </c>
-      <c r="I25" s="154">
-        <v>0</v>
-      </c>
-      <c r="J25" s="155">
+      <c r="H25" s="123">
+        <v>0</v>
+      </c>
+      <c r="I25" s="123">
+        <v>0</v>
+      </c>
+      <c r="J25" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2445,13 +2604,13 @@
       <c r="E26" s="94"/>
       <c r="F26" s="97"/>
       <c r="G26" s="100"/>
-      <c r="H26" s="154">
-        <v>0</v>
-      </c>
-      <c r="I26" s="154">
-        <v>0</v>
-      </c>
-      <c r="J26" s="155">
+      <c r="H26" s="123">
+        <v>0</v>
+      </c>
+      <c r="I26" s="123">
+        <v>0</v>
+      </c>
+      <c r="J26" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2466,13 +2625,13 @@
       <c r="E27" s="94"/>
       <c r="F27" s="97"/>
       <c r="G27" s="100"/>
-      <c r="H27" s="154">
-        <v>0</v>
-      </c>
-      <c r="I27" s="154">
-        <v>0</v>
-      </c>
-      <c r="J27" s="155">
+      <c r="H27" s="123">
+        <v>0</v>
+      </c>
+      <c r="I27" s="123">
+        <v>0</v>
+      </c>
+      <c r="J27" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2487,13 +2646,13 @@
       <c r="E28" s="94"/>
       <c r="F28" s="97"/>
       <c r="G28" s="100"/>
-      <c r="H28" s="154">
-        <v>0</v>
-      </c>
-      <c r="I28" s="154">
-        <v>0</v>
-      </c>
-      <c r="J28" s="155">
+      <c r="H28" s="123">
+        <v>0</v>
+      </c>
+      <c r="I28" s="123">
+        <v>0</v>
+      </c>
+      <c r="J28" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2508,13 +2667,13 @@
       <c r="E29" s="94"/>
       <c r="F29" s="97"/>
       <c r="G29" s="100"/>
-      <c r="H29" s="154">
-        <v>0</v>
-      </c>
-      <c r="I29" s="154">
-        <v>0</v>
-      </c>
-      <c r="J29" s="155">
+      <c r="H29" s="123">
+        <v>0</v>
+      </c>
+      <c r="I29" s="123">
+        <v>0</v>
+      </c>
+      <c r="J29" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2529,13 +2688,13 @@
       <c r="E30" s="95"/>
       <c r="F30" s="98"/>
       <c r="G30" s="101"/>
-      <c r="H30" s="156">
-        <v>0</v>
-      </c>
-      <c r="I30" s="156">
-        <v>0</v>
-      </c>
-      <c r="J30" s="157">
+      <c r="H30" s="125">
+        <v>0</v>
+      </c>
+      <c r="I30" s="125">
+        <v>0</v>
+      </c>
+      <c r="J30" s="126">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2616,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q50"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:H16"/>
+    <sheetView topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2649,18 +2808,18 @@
     </row>
     <row r="3" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
       <c r="M3" s="14"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
@@ -2696,10 +2855,10 @@
       <c r="I5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="152" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="127"/>
+      <c r="K5" s="152"/>
       <c r="L5" s="34" t="s">
         <v>36</v>
       </c>
@@ -2724,10 +2883,10 @@
       <c r="I6" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="128" t="s">
+      <c r="J6" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="128"/>
+      <c r="K6" s="153"/>
       <c r="L6" s="37">
         <f>16/25*100</f>
         <v>64</v>
@@ -2753,10 +2912,10 @@
       <c r="I7" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="129" t="s">
+      <c r="J7" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="129"/>
+      <c r="K7" s="147"/>
       <c r="L7" s="42">
         <f>15/25*100</f>
         <v>60</v>
@@ -2782,10 +2941,10 @@
       <c r="I8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="129" t="s">
+      <c r="J8" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="129"/>
+      <c r="K8" s="147"/>
       <c r="L8" s="42">
         <f>12/25*100</f>
         <v>48</v>
@@ -2811,10 +2970,10 @@
       <c r="I9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="129" t="s">
+      <c r="J9" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="129"/>
+      <c r="K9" s="147"/>
       <c r="L9" s="42">
         <f>8/25*100</f>
         <v>32</v>
@@ -2840,10 +2999,10 @@
       <c r="I10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="130" t="s">
+      <c r="J10" s="148" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="130"/>
+      <c r="K10" s="148"/>
       <c r="L10" s="47">
         <f>5/25*100</f>
         <v>20</v>
@@ -2889,10 +3048,10 @@
       <c r="C13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="131" t="s">
+      <c r="D13" s="149" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="149"/>
       <c r="F13" s="51" t="s">
         <v>54</v>
       </c>
@@ -2916,25 +3075,25 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="53" t="str">
         <f>CONCATENATE($B$13,Matriz!B16)</f>
         <v>R1</v>
       </c>
-      <c r="D14" s="132" t="str">
+      <c r="D14" s="150" t="str">
         <f>Matriz!E16</f>
-        <v>Daño en el equipo de cómputo</v>
-      </c>
-      <c r="E14" s="132"/>
+        <v>Organización ineficiente</v>
+      </c>
+      <c r="E14" s="150"/>
       <c r="F14" s="54" t="str">
         <f>Matriz!F16</f>
-        <v>Mala instalación eléctrica</v>
+        <v>Mala organización del equipo de trabajo</v>
       </c>
       <c r="G14" s="55"/>
       <c r="H14" s="54">
         <f>Matriz!H16</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I14" s="54">
         <f>Matriz!I16</f>
@@ -2942,7 +3101,7 @@
       </c>
       <c r="J14" s="56">
         <f t="shared" ref="J14:J28" si="0">H14*I14</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K14" s="56" t="str">
         <f t="shared" ref="K14:K28" si="1">IF(J14&lt;5,"MUY BAJO",IF( AND(J14&gt;=5,J14&lt;8),"BAJO",IF(AND(J14&gt;=8,J14&lt;=12),"MODERADO",IF(AND(J14&gt;=12,J14&lt;=15),"ALTO","MUY ALTO"))))</f>
@@ -2950,26 +3109,28 @@
       </c>
       <c r="L14" s="57">
         <f t="shared" ref="L14:L28" si="2">J14/25*100</f>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="61.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B17)</f>
         <v>R2</v>
       </c>
-      <c r="D15" s="133" t="str">
+      <c r="D15" s="143" t="str">
         <f>Matriz!E17</f>
-        <v>Tiempos incongruentes y fechas mal planeadas.</v>
-      </c>
-      <c r="E15" s="133"/>
+        <v>Tiempos incongruentes y fechas mal planeadas</v>
+      </c>
+      <c r="E15" s="143"/>
       <c r="F15" s="58" t="str">
         <f>Matriz!F17</f>
         <v xml:space="preserve">Mala planeación del proyecto </v>
       </c>
-      <c r="G15" s="59"/>
+      <c r="G15" s="117" t="s">
+        <v>88</v>
+      </c>
       <c r="H15" s="58">
         <f>Matriz!H17</f>
         <v>3</v>
@@ -2992,155 +3153,164 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B18)</f>
         <v>R3</v>
       </c>
-      <c r="D16" s="133">
+      <c r="D16" s="143" t="str">
         <f>Matriz!E18</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="133"/>
-      <c r="F16" s="58">
+        <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
+      </c>
+      <c r="E16" s="143"/>
+      <c r="F16" s="117" t="str">
         <f>Matriz!F18</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="59"/>
+        <v>Mala comunicación con el cliente</v>
+      </c>
+      <c r="G16" s="117" t="s">
+        <v>114</v>
+      </c>
       <c r="H16" s="58">
         <f>Matriz!H18</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I16" s="58">
         <f>Matriz!I18</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J16" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K16" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>MUY BAJO</v>
+        <v>MODERADO</v>
       </c>
       <c r="L16" s="61">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="86.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B19)</f>
         <v>R4</v>
       </c>
-      <c r="D17" s="133">
+      <c r="D17" s="143" t="str">
         <f>Matriz!E19</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="133"/>
-      <c r="F17" s="58">
+        <v>Incorrecta interpretación de las ventanas e interfaces</v>
+      </c>
+      <c r="E17" s="143"/>
+      <c r="F17" s="117" t="str">
         <f>Matriz!F19</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="59"/>
+        <v>Mal entendimiento de los requerimientos</v>
+      </c>
+      <c r="G17" s="117" t="s">
+        <v>98</v>
+      </c>
       <c r="H17" s="58">
         <f>Matriz!H19</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" s="58">
         <f>Matriz!I19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K17" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>MUY BAJO</v>
+        <v>BAJO</v>
       </c>
       <c r="L17" s="61">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B20)</f>
         <v>R5</v>
       </c>
-      <c r="D18" s="133">
+      <c r="D18" s="143" t="str">
         <f>Matriz!E20</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="133"/>
-      <c r="F18" s="58">
+        <v>Incorrecta definición y estructura de los datos</v>
+      </c>
+      <c r="E18" s="143"/>
+      <c r="F18" s="58" t="str">
         <f>Matriz!F20</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="59"/>
+        <v>Mal entendimiento de las
+relaciones y dependencias del producto</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>115</v>
+      </c>
       <c r="H18" s="58">
         <f>Matriz!H20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I18" s="58">
         <f>Matriz!I20</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J18" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K18" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>MUY BAJO</v>
+        <v>MODERADO</v>
       </c>
       <c r="L18" s="61">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="2:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="44" t="str">
         <f>CONCATENATE($B$13,Matriz!B21)</f>
         <v>R6</v>
       </c>
-      <c r="D19" s="133">
+      <c r="D19" s="143" t="str">
         <f>Matriz!E21</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="133"/>
-      <c r="F19" s="58">
+        <v>Pruebas ineficientes</v>
+      </c>
+      <c r="E19" s="143"/>
+      <c r="F19" s="58" t="str">
         <f>Matriz!F21</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="59"/>
+        <v>Mala realización de pruebas</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>108</v>
+      </c>
       <c r="H19" s="58">
         <f>Matriz!H21</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I19" s="58">
         <f>Matriz!I21</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J19" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K19" s="60" t="str">
         <f t="shared" si="1"/>
-        <v>MUY BAJO</v>
+        <v>ALTO</v>
       </c>
       <c r="L19" s="61">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M19" s="14"/>
     </row>
@@ -3150,11 +3320,11 @@
         <f>CONCATENATE($B$13,Matriz!B22)</f>
         <v>R7</v>
       </c>
-      <c r="D20" s="133">
+      <c r="D20" s="143">
         <f>Matriz!E22</f>
         <v>0</v>
       </c>
-      <c r="E20" s="133"/>
+      <c r="E20" s="143"/>
       <c r="F20" s="58">
         <f>Matriz!F22</f>
         <v>0</v>
@@ -3188,11 +3358,11 @@
         <f>CONCATENATE($B$13,Matriz!B23)</f>
         <v>R8</v>
       </c>
-      <c r="D21" s="133">
+      <c r="D21" s="143">
         <f>Matriz!E23</f>
         <v>0</v>
       </c>
-      <c r="E21" s="133"/>
+      <c r="E21" s="143"/>
       <c r="F21" s="58">
         <f>Matriz!F23</f>
         <v>0</v>
@@ -3226,11 +3396,11 @@
         <f>CONCATENATE($B$13,Matriz!B24)</f>
         <v>R9</v>
       </c>
-      <c r="D22" s="133">
+      <c r="D22" s="143">
         <f>Matriz!E24</f>
         <v>0</v>
       </c>
-      <c r="E22" s="133"/>
+      <c r="E22" s="143"/>
       <c r="F22" s="58">
         <f>Matriz!F24</f>
         <v>0</v>
@@ -3264,11 +3434,11 @@
         <f>CONCATENATE($B$13,Matriz!B25)</f>
         <v>R10</v>
       </c>
-      <c r="D23" s="133">
+      <c r="D23" s="143">
         <f>Matriz!E25</f>
         <v>0</v>
       </c>
-      <c r="E23" s="133"/>
+      <c r="E23" s="143"/>
       <c r="F23" s="58">
         <f>Matriz!F25</f>
         <v>0</v>
@@ -3302,11 +3472,11 @@
         <f>CONCATENATE($B$13,Matriz!B26)</f>
         <v>R11</v>
       </c>
-      <c r="D24" s="133">
+      <c r="D24" s="143">
         <f>Matriz!E26</f>
         <v>0</v>
       </c>
-      <c r="E24" s="133"/>
+      <c r="E24" s="143"/>
       <c r="F24" s="58">
         <f>Matriz!F26</f>
         <v>0</v>
@@ -3340,11 +3510,11 @@
         <f>CONCATENATE($B$13,Matriz!B27)</f>
         <v>R12</v>
       </c>
-      <c r="D25" s="133">
+      <c r="D25" s="143">
         <f>Matriz!E27</f>
         <v>0</v>
       </c>
-      <c r="E25" s="133"/>
+      <c r="E25" s="143"/>
       <c r="F25" s="58">
         <f>Matriz!F27</f>
         <v>0</v>
@@ -3378,11 +3548,11 @@
         <f>CONCATENATE($B$13,Matriz!B28)</f>
         <v>R13</v>
       </c>
-      <c r="D26" s="133">
+      <c r="D26" s="143">
         <f>Matriz!E28</f>
         <v>0</v>
       </c>
-      <c r="E26" s="133"/>
+      <c r="E26" s="143"/>
       <c r="F26" s="58">
         <f>Matriz!F28</f>
         <v>0</v>
@@ -3416,11 +3586,11 @@
         <f>CONCATENATE($B$13,Matriz!B29)</f>
         <v>R14</v>
       </c>
-      <c r="D27" s="133">
+      <c r="D27" s="143">
         <f>Matriz!E29</f>
         <v>0</v>
       </c>
-      <c r="E27" s="133"/>
+      <c r="E27" s="143"/>
       <c r="F27" s="58">
         <f>Matriz!F29</f>
         <v>0</v>
@@ -3454,11 +3624,11 @@
         <f>CONCATENATE($B$13,Matriz!B30)</f>
         <v>R15</v>
       </c>
-      <c r="D28" s="133">
+      <c r="D28" s="143">
         <f>Matriz!E30</f>
         <v>0</v>
       </c>
-      <c r="E28" s="133"/>
+      <c r="E28" s="143"/>
       <c r="F28" s="58">
         <f>Matriz!F30</f>
         <v>0</v>
@@ -3501,20 +3671,20 @@
       <c r="M29" s="14"/>
     </row>
     <row r="30" spans="2:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="134" t="s">
+      <c r="B30" s="144" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="134"/>
-      <c r="D30" s="134"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="134"/>
-      <c r="I30" s="134"/>
-      <c r="J30" s="134"/>
-      <c r="K30" s="134"/>
-      <c r="L30" s="134"/>
-      <c r="M30" s="134"/>
+      <c r="C30" s="144"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="144"/>
+      <c r="J30" s="144"/>
+      <c r="K30" s="144"/>
+      <c r="L30" s="144"/>
+      <c r="M30" s="144"/>
     </row>
     <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
@@ -3535,10 +3705,10 @@
       <c r="C32" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="135" t="s">
+      <c r="D32" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="135"/>
+      <c r="E32" s="145"/>
       <c r="F32" s="63" t="s">
         <v>62</v>
       </c>
@@ -3554,64 +3724,66 @@
       <c r="J32" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="K32" s="136" t="s">
+      <c r="K32" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="L32" s="136"/>
+      <c r="L32" s="146"/>
       <c r="M32" s="14"/>
     </row>
-    <row r="33" spans="2:13" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="163.80000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="64" t="str">
         <f t="shared" ref="C33:D47" si="3">C14</f>
         <v>R1</v>
       </c>
-      <c r="D33" s="137" t="str">
+      <c r="D33" s="140" t="str">
         <f t="shared" si="3"/>
-        <v>Daño en el equipo de cómputo</v>
-      </c>
-      <c r="E33" s="137"/>
+        <v>Organización ineficiente</v>
+      </c>
+      <c r="E33" s="140"/>
       <c r="F33" s="66" t="str">
         <f t="shared" ref="F33:F47" si="4">K14</f>
         <v>MODERADO</v>
       </c>
       <c r="G33" s="65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H33" s="65" t="str">
         <f>Matriz!K16</f>
-        <v>Verificar la instalación electrica del local y utilizar no breaks</v>
+        <v>•Definir nomenclatura para cada archivo sujeto con un control de versión
+•Crear un repositorio en la nube para subir y bajar actualizaciónes</v>
       </c>
       <c r="I33" s="65" t="s">
         <v>67</v>
       </c>
       <c r="J33" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="K33" s="138" t="str">
+        <v>83</v>
+      </c>
+      <c r="K33" s="141" t="str">
         <f>Matriz!K16</f>
-        <v>Verificar la instalación electrica del local y utilizar no breaks</v>
-      </c>
-      <c r="L33" s="138"/>
+        <v>•Definir nomenclatura para cada archivo sujeto con un control de versión
+•Crear un repositorio en la nube para subir y bajar actualizaciónes</v>
+      </c>
+      <c r="L33" s="141"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="2:13" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R2</v>
       </c>
-      <c r="D34" s="139" t="str">
+      <c r="D34" s="142" t="str">
         <f t="shared" si="3"/>
-        <v>Tiempos incongruentes y fechas mal planeadas.</v>
-      </c>
-      <c r="E34" s="139"/>
+        <v>Tiempos incongruentes y fechas mal planeadas</v>
+      </c>
+      <c r="E34" s="142"/>
       <c r="F34" s="68" t="str">
         <f t="shared" si="4"/>
         <v>MODERADO</v>
       </c>
       <c r="G34" s="69" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H34" s="89" t="str">
         <f>Matriz!K17</f>
@@ -3621,137 +3793,157 @@
         <v>67</v>
       </c>
       <c r="J34" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="K34" s="140" t="str">
+        <v>83</v>
+      </c>
+      <c r="K34" s="139" t="str">
         <f>Matriz!K17</f>
         <v>Revisar actividades con fechas y ajustarlos a tiempos del proyecto.</v>
       </c>
-      <c r="L34" s="140"/>
+      <c r="L34" s="139"/>
       <c r="M34" s="14"/>
     </row>
-    <row r="35" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="125.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
       <c r="C35" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R3</v>
       </c>
-      <c r="D35" s="141">
+      <c r="D35" s="138" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="141"/>
+        <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
+      </c>
+      <c r="E35" s="138"/>
       <c r="F35" s="71" t="str">
         <f t="shared" si="4"/>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="G35" s="70"/>
-      <c r="H35" s="89">
+        <v>MODERADO</v>
+      </c>
+      <c r="G35" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="89" t="str">
         <f>Matriz!K18</f>
-        <v>0</v>
+        <v xml:space="preserve">Acomplar los nuevos cambios o requetimientos a los existentes de forma clara y completa para cumplir la funcionalidad planeada </v>
       </c>
       <c r="I35" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="J35" s="70"/>
-      <c r="K35" s="140">
+      <c r="J35" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" s="139" t="str">
         <f>Matriz!K18</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="140"/>
+        <v xml:space="preserve">Acomplar los nuevos cambios o requetimientos a los existentes de forma clara y completa para cumplir la funcionalidad planeada </v>
+      </c>
+      <c r="L35" s="139"/>
       <c r="M35" s="14"/>
     </row>
-    <row r="36" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
       <c r="C36" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R4</v>
       </c>
-      <c r="D36" s="141">
+      <c r="D36" s="138" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="141"/>
+        <v>Incorrecta interpretación de las ventanas e interfaces</v>
+      </c>
+      <c r="E36" s="138"/>
       <c r="F36" s="68" t="str">
         <f t="shared" si="4"/>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="G36" s="69"/>
-      <c r="H36" s="89">
+        <v>BAJO</v>
+      </c>
+      <c r="G36" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="89" t="str">
         <f>Matriz!K19</f>
-        <v>0</v>
+        <v>Rediseñar las interfaces con base  a las especificaciónes de requerimientos</v>
       </c>
       <c r="I36" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="J36" s="69"/>
-      <c r="K36" s="140">
+      <c r="J36" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="K36" s="139" t="str">
         <f>Matriz!K19</f>
-        <v>0</v>
-      </c>
-      <c r="L36" s="140"/>
+        <v>Rediseñar las interfaces con base  a las especificaciónes de requerimientos</v>
+      </c>
+      <c r="L36" s="139"/>
       <c r="M36" s="14"/>
     </row>
-    <row r="37" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" ht="147" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
       <c r="C37" s="67" t="str">
         <f t="shared" si="3"/>
         <v>R5</v>
       </c>
-      <c r="D37" s="141">
+      <c r="D37" s="138" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="141"/>
+        <v>Incorrecta definición y estructura de los datos</v>
+      </c>
+      <c r="E37" s="138"/>
       <c r="F37" s="71" t="str">
         <f t="shared" si="4"/>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="G37" s="70"/>
-      <c r="H37" s="89">
+        <v>MODERADO</v>
+      </c>
+      <c r="G37" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="89" t="str">
         <f>Matriz!K20</f>
-        <v>0</v>
+        <v>Definir la arquitectura lógica y las relaciones correctas con base a los procesos de la empresa</v>
       </c>
       <c r="I37" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="70"/>
-      <c r="K37" s="140">
+      <c r="J37" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="K37" s="139" t="str">
         <f>Matriz!K20</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="140"/>
+        <v>Definir la arquitectura lógica y las relaciones correctas con base a los procesos de la empresa</v>
+      </c>
+      <c r="L37" s="139"/>
       <c r="M37" s="14"/>
     </row>
-    <row r="38" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="194.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
       <c r="C38" s="72" t="str">
         <f t="shared" si="3"/>
         <v>R6</v>
       </c>
-      <c r="D38" s="142">
+      <c r="D38" s="136" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="142"/>
+        <v>Pruebas ineficientes</v>
+      </c>
+      <c r="E38" s="136"/>
       <c r="F38" s="73" t="str">
         <f t="shared" si="4"/>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="G38" s="74"/>
-      <c r="H38" s="89">
+        <v>ALTO</v>
+      </c>
+      <c r="G38" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" s="89" t="str">
         <f>Matriz!K21</f>
-        <v>0</v>
+        <v>•Realizar pruebas de cada modulo de la aplicación detalladamente
+•Darle seguimiento a cada falla encontrado
+•Volver a probar los módulos donde hubieron fallas</v>
       </c>
       <c r="I38" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="J38" s="74"/>
-      <c r="K38" s="143">
+      <c r="J38" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" s="137" t="str">
         <f>Matriz!K21</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="143"/>
+        <v>•Realizar pruebas de cada modulo de la aplicación detalladamente
+•Darle seguimiento a cada falla encontrado
+•Volver a probar los módulos donde hubieron fallas</v>
+      </c>
+      <c r="L38" s="137"/>
       <c r="M38" s="14"/>
     </row>
     <row r="39" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3760,11 +3952,11 @@
         <f t="shared" si="3"/>
         <v>R7</v>
       </c>
-      <c r="D39" s="142">
+      <c r="D39" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E39" s="142"/>
+      <c r="E39" s="136"/>
       <c r="F39" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3778,11 +3970,11 @@
         <v>67</v>
       </c>
       <c r="J39" s="74"/>
-      <c r="K39" s="143">
+      <c r="K39" s="137">
         <f>Matriz!K22</f>
         <v>0</v>
       </c>
-      <c r="L39" s="143"/>
+      <c r="L39" s="137"/>
       <c r="M39" s="14"/>
     </row>
     <row r="40" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3791,11 +3983,11 @@
         <f t="shared" si="3"/>
         <v>R8</v>
       </c>
-      <c r="D40" s="142">
+      <c r="D40" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E40" s="142"/>
+      <c r="E40" s="136"/>
       <c r="F40" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3809,11 +4001,11 @@
         <v>67</v>
       </c>
       <c r="J40" s="74"/>
-      <c r="K40" s="143">
+      <c r="K40" s="137">
         <f>Matriz!K23</f>
         <v>0</v>
       </c>
-      <c r="L40" s="143"/>
+      <c r="L40" s="137"/>
       <c r="M40" s="14"/>
     </row>
     <row r="41" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3822,11 +4014,11 @@
         <f t="shared" si="3"/>
         <v>R9</v>
       </c>
-      <c r="D41" s="142">
+      <c r="D41" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E41" s="142"/>
+      <c r="E41" s="136"/>
       <c r="F41" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3840,11 +4032,11 @@
         <v>67</v>
       </c>
       <c r="J41" s="74"/>
-      <c r="K41" s="143">
+      <c r="K41" s="137">
         <f>Matriz!K24</f>
         <v>0</v>
       </c>
-      <c r="L41" s="143"/>
+      <c r="L41" s="137"/>
       <c r="M41" s="14"/>
     </row>
     <row r="42" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3853,11 +4045,11 @@
         <f t="shared" si="3"/>
         <v>R10</v>
       </c>
-      <c r="D42" s="142">
+      <c r="D42" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E42" s="142"/>
+      <c r="E42" s="136"/>
       <c r="F42" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3871,11 +4063,11 @@
         <v>67</v>
       </c>
       <c r="J42" s="74"/>
-      <c r="K42" s="143">
+      <c r="K42" s="137">
         <f>Matriz!K25</f>
         <v>0</v>
       </c>
-      <c r="L42" s="143"/>
+      <c r="L42" s="137"/>
       <c r="M42" s="14"/>
     </row>
     <row r="43" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3884,11 +4076,11 @@
         <f t="shared" si="3"/>
         <v>R11</v>
       </c>
-      <c r="D43" s="142">
+      <c r="D43" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E43" s="142"/>
+      <c r="E43" s="136"/>
       <c r="F43" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3902,11 +4094,11 @@
         <v>67</v>
       </c>
       <c r="J43" s="74"/>
-      <c r="K43" s="143">
+      <c r="K43" s="137">
         <f>Matriz!K26</f>
         <v>0</v>
       </c>
-      <c r="L43" s="143"/>
+      <c r="L43" s="137"/>
       <c r="M43" s="14"/>
     </row>
     <row r="44" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3915,11 +4107,11 @@
         <f t="shared" si="3"/>
         <v>R12</v>
       </c>
-      <c r="D44" s="142">
+      <c r="D44" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E44" s="142"/>
+      <c r="E44" s="136"/>
       <c r="F44" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3933,11 +4125,11 @@
         <v>67</v>
       </c>
       <c r="J44" s="74"/>
-      <c r="K44" s="143">
+      <c r="K44" s="137">
         <f>Matriz!K27</f>
         <v>0</v>
       </c>
-      <c r="L44" s="143"/>
+      <c r="L44" s="137"/>
       <c r="M44" s="14"/>
     </row>
     <row r="45" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3946,11 +4138,11 @@
         <f t="shared" si="3"/>
         <v>R13</v>
       </c>
-      <c r="D45" s="142">
+      <c r="D45" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E45" s="142"/>
+      <c r="E45" s="136"/>
       <c r="F45" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3964,11 +4156,11 @@
         <v>67</v>
       </c>
       <c r="J45" s="74"/>
-      <c r="K45" s="143">
+      <c r="K45" s="137">
         <f>Matriz!K28</f>
         <v>0</v>
       </c>
-      <c r="L45" s="143"/>
+      <c r="L45" s="137"/>
       <c r="M45" s="14"/>
     </row>
     <row r="46" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3977,11 +4169,11 @@
         <f t="shared" si="3"/>
         <v>R14</v>
       </c>
-      <c r="D46" s="142">
+      <c r="D46" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E46" s="142"/>
+      <c r="E46" s="136"/>
       <c r="F46" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -3995,11 +4187,11 @@
         <v>67</v>
       </c>
       <c r="J46" s="74"/>
-      <c r="K46" s="143">
+      <c r="K46" s="137">
         <f>Matriz!K29</f>
         <v>0</v>
       </c>
-      <c r="L46" s="143"/>
+      <c r="L46" s="137"/>
       <c r="M46" s="14"/>
     </row>
     <row r="47" spans="2:13" ht="27.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4008,11 +4200,11 @@
         <f t="shared" si="3"/>
         <v>R15</v>
       </c>
-      <c r="D47" s="142">
+      <c r="D47" s="136">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E47" s="142"/>
+      <c r="E47" s="136"/>
       <c r="F47" s="73" t="str">
         <f t="shared" si="4"/>
         <v>MUY BAJO</v>
@@ -4026,11 +4218,11 @@
         <v>67</v>
       </c>
       <c r="J47" s="74"/>
-      <c r="K47" s="143">
+      <c r="K47" s="137">
         <f>Matriz!K30</f>
         <v>0</v>
       </c>
-      <c r="L47" s="143"/>
+      <c r="L47" s="137"/>
       <c r="M47" s="14"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
@@ -4077,62 +4269,62 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="C3:L3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K44:L44"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="K47:L47"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="L14:L28">
     <cfRule type="colorScale" priority="2">
@@ -4187,7 +4379,7 @@
   <dimension ref="C4:O25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:N9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4202,21 +4394,21 @@
   <sheetData>
     <row r="4" spans="3:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="3:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="144" t="s">
+      <c r="C5" s="155" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="144"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
+      <c r="K5" s="155"/>
+      <c r="L5" s="155"/>
+      <c r="M5" s="155"/>
+      <c r="N5" s="155"/>
+      <c r="O5" s="155"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="12"/>
@@ -4238,10 +4430,10 @@
       <c r="D7" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="156" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="145"/>
+      <c r="F7" s="156"/>
       <c r="G7" s="78" t="s">
         <v>62</v>
       </c>
@@ -4260,23 +4452,23 @@
       <c r="L7" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="145" t="s">
+      <c r="M7" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="145"/>
+      <c r="N7" s="156"/>
       <c r="O7" s="14"/>
     </row>
-    <row r="8" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="12"/>
       <c r="D8" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C33</f>
         <v>R1</v>
       </c>
-      <c r="E8" s="146" t="str">
+      <c r="E8" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D33</f>
-        <v>Daño en el equipo de cómputo</v>
-      </c>
-      <c r="F8" s="146"/>
+        <v>Organización ineficiente</v>
+      </c>
+      <c r="F8" s="154"/>
       <c r="G8" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F33</f>
         <v>MODERADO</v>
@@ -4287,33 +4479,36 @@
       </c>
       <c r="I8" s="80" t="str">
         <f>Matriz!K16</f>
-        <v>Verificar la instalación electrica del local y utilizar no breaks</v>
+        <v>•Definir nomenclatura para cada archivo sujeto con un control de versión
+•Crear un repositorio en la nube para subir y bajar actualizaciónes</v>
       </c>
       <c r="J8" s="82" t="s">
         <v>74</v>
       </c>
       <c r="K8" s="116">
-        <v>43651</v>
+        <v>43565</v>
       </c>
       <c r="L8" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J33</f>
         <v>Project Manager</v>
       </c>
-      <c r="M8" s="146"/>
-      <c r="N8" s="146"/>
+      <c r="M8" s="154" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="154"/>
       <c r="O8" s="14"/>
     </row>
-    <row r="9" spans="3:15" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12"/>
       <c r="D9" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C34</f>
         <v>R2</v>
       </c>
-      <c r="E9" s="146" t="str">
+      <c r="E9" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D34</f>
-        <v>Tiempos incongruentes y fechas mal planeadas.</v>
-      </c>
-      <c r="F9" s="146"/>
+        <v>Tiempos incongruentes y fechas mal planeadas</v>
+      </c>
+      <c r="F9" s="154"/>
       <c r="G9" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F34</f>
         <v>MODERADO</v>
@@ -4336,142 +4531,158 @@
         <f>'Cualitativo y Cuantitativo'!J34</f>
         <v>Project Manager</v>
       </c>
-      <c r="M9" s="146" t="s">
-        <v>92</v>
-      </c>
-      <c r="N9" s="146"/>
+      <c r="M9" s="154" t="s">
+        <v>118</v>
+      </c>
+      <c r="N9" s="154"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="12"/>
       <c r="D10" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C35</f>
         <v>R3</v>
       </c>
-      <c r="E10" s="146">
+      <c r="E10" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D35</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="146"/>
+        <v>Cambios regulares y nuevos añadidos a los requerimientos</v>
+      </c>
+      <c r="F10" s="154"/>
       <c r="G10" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F35</f>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="H10" s="80">
+        <v>MODERADO</v>
+      </c>
+      <c r="H10" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J35</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="80">
+        <v>Project Manager</v>
+      </c>
+      <c r="I10" s="118" t="str">
         <f>Matriz!K18</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="82"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80">
+        <v xml:space="preserve">Acomplar los nuevos cambios o requetimientos a los existentes de forma clara y completa para cumplir la funcionalidad planeada </v>
+      </c>
+      <c r="J10" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="116">
+        <v>43631</v>
+      </c>
+      <c r="L10" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J35</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="146"/>
-      <c r="N10" s="146"/>
+        <v>Project Manager</v>
+      </c>
+      <c r="M10" s="154" t="s">
+        <v>117</v>
+      </c>
+      <c r="N10" s="154"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" ht="92.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="12"/>
       <c r="D11" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C36</f>
         <v>R4</v>
       </c>
-      <c r="E11" s="146">
+      <c r="E11" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D36</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="146"/>
+        <v>Incorrecta interpretación de las ventanas e interfaces</v>
+      </c>
+      <c r="F11" s="154"/>
       <c r="G11" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F36</f>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="H11" s="80">
-        <f>'Cualitativo y Cuantitativo'!J36</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="80">
+        <v>BAJO</v>
+      </c>
+      <c r="H11" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="80" t="str">
         <f>Matriz!K19</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="82"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="80">
-        <f>'Cualitativo y Cuantitativo'!J36</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="146"/>
-      <c r="N11" s="146"/>
+        <v>Rediseñar las interfaces con base  a las especificaciónes de requerimientos</v>
+      </c>
+      <c r="J11" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="116">
+        <v>43642</v>
+      </c>
+      <c r="L11" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="154"/>
+      <c r="N11" s="154"/>
       <c r="O11" s="14"/>
     </row>
-    <row r="12" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
       <c r="D12" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C37</f>
         <v>R5</v>
       </c>
-      <c r="E12" s="146">
+      <c r="E12" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D37</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="146"/>
+        <v>Incorrecta definición y estructura de los datos</v>
+      </c>
+      <c r="F12" s="154"/>
       <c r="G12" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F37</f>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="H12" s="80">
+        <v>MODERADO</v>
+      </c>
+      <c r="H12" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J37</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="80">
+        <v>Project Manager</v>
+      </c>
+      <c r="I12" s="80" t="str">
         <f>Matriz!K20</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="82"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80">
+        <v>Definir la arquitectura lógica y las relaciones correctas con base a los procesos de la empresa</v>
+      </c>
+      <c r="J12" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="116">
+        <v>43645</v>
+      </c>
+      <c r="L12" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J37</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="146"/>
-      <c r="N12" s="146"/>
+        <v>Project Manager</v>
+      </c>
+      <c r="M12" s="154" t="s">
+        <v>119</v>
+      </c>
+      <c r="N12" s="154"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="12"/>
       <c r="D13" s="79" t="str">
         <f>'Cualitativo y Cuantitativo'!C38</f>
         <v>R6</v>
       </c>
-      <c r="E13" s="146">
+      <c r="E13" s="154" t="str">
         <f>'Cualitativo y Cuantitativo'!D38</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="146"/>
+        <v>Pruebas ineficientes</v>
+      </c>
+      <c r="F13" s="154"/>
       <c r="G13" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F38</f>
-        <v>MUY BAJO</v>
-      </c>
-      <c r="H13" s="80">
+        <v>ALTO</v>
+      </c>
+      <c r="H13" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J38</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="80">
+        <v>Análista</v>
+      </c>
+      <c r="I13" s="80" t="str">
         <f>Matriz!K21</f>
-        <v>0</v>
+        <v>•Realizar pruebas de cada modulo de la aplicación detalladamente
+•Darle seguimiento a cada falla encontrado
+•Volver a probar los módulos donde hubieron fallas</v>
       </c>
       <c r="J13" s="82"/>
       <c r="K13" s="80"/>
-      <c r="L13" s="80">
+      <c r="L13" s="80" t="str">
         <f>'Cualitativo y Cuantitativo'!J38</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="146"/>
-      <c r="N13" s="146"/>
+        <v>Análista</v>
+      </c>
+      <c r="M13" s="154"/>
+      <c r="N13" s="154"/>
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4480,11 +4691,11 @@
         <f>'Cualitativo y Cuantitativo'!C39</f>
         <v>R7</v>
       </c>
-      <c r="E14" s="146">
+      <c r="E14" s="154">
         <f>'Cualitativo y Cuantitativo'!D39</f>
         <v>0</v>
       </c>
-      <c r="F14" s="146"/>
+      <c r="F14" s="154"/>
       <c r="G14" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F39</f>
         <v>MUY BAJO</v>
@@ -4503,8 +4714,8 @@
         <f>'Cualitativo y Cuantitativo'!J39</f>
         <v>0</v>
       </c>
-      <c r="M14" s="146"/>
-      <c r="N14" s="146"/>
+      <c r="M14" s="154"/>
+      <c r="N14" s="154"/>
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4513,11 +4724,11 @@
         <f>'Cualitativo y Cuantitativo'!C40</f>
         <v>R8</v>
       </c>
-      <c r="E15" s="146">
+      <c r="E15" s="154">
         <f>'Cualitativo y Cuantitativo'!D40</f>
         <v>0</v>
       </c>
-      <c r="F15" s="146"/>
+      <c r="F15" s="154"/>
       <c r="G15" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F40</f>
         <v>MUY BAJO</v>
@@ -4536,8 +4747,8 @@
         <f>'Cualitativo y Cuantitativo'!J40</f>
         <v>0</v>
       </c>
-      <c r="M15" s="146"/>
-      <c r="N15" s="146"/>
+      <c r="M15" s="154"/>
+      <c r="N15" s="154"/>
       <c r="O15" s="14"/>
     </row>
     <row r="16" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4546,11 +4757,11 @@
         <f>'Cualitativo y Cuantitativo'!C41</f>
         <v>R9</v>
       </c>
-      <c r="E16" s="146">
+      <c r="E16" s="154">
         <f>'Cualitativo y Cuantitativo'!D41</f>
         <v>0</v>
       </c>
-      <c r="F16" s="146"/>
+      <c r="F16" s="154"/>
       <c r="G16" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F41</f>
         <v>MUY BAJO</v>
@@ -4569,8 +4780,8 @@
         <f>'Cualitativo y Cuantitativo'!J41</f>
         <v>0</v>
       </c>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
+      <c r="M16" s="154"/>
+      <c r="N16" s="154"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4579,11 +4790,11 @@
         <f>'Cualitativo y Cuantitativo'!C42</f>
         <v>R10</v>
       </c>
-      <c r="E17" s="146">
+      <c r="E17" s="154">
         <f>'Cualitativo y Cuantitativo'!D42</f>
         <v>0</v>
       </c>
-      <c r="F17" s="146"/>
+      <c r="F17" s="154"/>
       <c r="G17" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F42</f>
         <v>MUY BAJO</v>
@@ -4602,8 +4813,8 @@
         <f>'Cualitativo y Cuantitativo'!J42</f>
         <v>0</v>
       </c>
-      <c r="M17" s="146"/>
-      <c r="N17" s="146"/>
+      <c r="M17" s="154"/>
+      <c r="N17" s="154"/>
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4612,11 +4823,11 @@
         <f>'Cualitativo y Cuantitativo'!C43</f>
         <v>R11</v>
       </c>
-      <c r="E18" s="146">
+      <c r="E18" s="154">
         <f>'Cualitativo y Cuantitativo'!D43</f>
         <v>0</v>
       </c>
-      <c r="F18" s="146"/>
+      <c r="F18" s="154"/>
       <c r="G18" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F43</f>
         <v>MUY BAJO</v>
@@ -4635,8 +4846,8 @@
         <f>'Cualitativo y Cuantitativo'!J43</f>
         <v>0</v>
       </c>
-      <c r="M18" s="146"/>
-      <c r="N18" s="146"/>
+      <c r="M18" s="154"/>
+      <c r="N18" s="154"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4645,11 +4856,11 @@
         <f>'Cualitativo y Cuantitativo'!C44</f>
         <v>R12</v>
       </c>
-      <c r="E19" s="146">
+      <c r="E19" s="154">
         <f>'Cualitativo y Cuantitativo'!D44</f>
         <v>0</v>
       </c>
-      <c r="F19" s="146"/>
+      <c r="F19" s="154"/>
       <c r="G19" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F44</f>
         <v>MUY BAJO</v>
@@ -4668,8 +4879,8 @@
         <f>'Cualitativo y Cuantitativo'!J44</f>
         <v>0</v>
       </c>
-      <c r="M19" s="146"/>
-      <c r="N19" s="146"/>
+      <c r="M19" s="154"/>
+      <c r="N19" s="154"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4678,11 +4889,11 @@
         <f>'Cualitativo y Cuantitativo'!C45</f>
         <v>R13</v>
       </c>
-      <c r="E20" s="146">
+      <c r="E20" s="154">
         <f>'Cualitativo y Cuantitativo'!D45</f>
         <v>0</v>
       </c>
-      <c r="F20" s="146"/>
+      <c r="F20" s="154"/>
       <c r="G20" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F45</f>
         <v>MUY BAJO</v>
@@ -4701,8 +4912,8 @@
         <f>'Cualitativo y Cuantitativo'!J45</f>
         <v>0</v>
       </c>
-      <c r="M20" s="146"/>
-      <c r="N20" s="146"/>
+      <c r="M20" s="154"/>
+      <c r="N20" s="154"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4711,11 +4922,11 @@
         <f>'Cualitativo y Cuantitativo'!C46</f>
         <v>R14</v>
       </c>
-      <c r="E21" s="146">
+      <c r="E21" s="154">
         <f>'Cualitativo y Cuantitativo'!D46</f>
         <v>0</v>
       </c>
-      <c r="F21" s="146"/>
+      <c r="F21" s="154"/>
       <c r="G21" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F46</f>
         <v>MUY BAJO</v>
@@ -4734,8 +4945,8 @@
         <f>'Cualitativo y Cuantitativo'!J46</f>
         <v>0</v>
       </c>
-      <c r="M21" s="146"/>
-      <c r="N21" s="146"/>
+      <c r="M21" s="154"/>
+      <c r="N21" s="154"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="3:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -4744,11 +4955,11 @@
         <f>'Cualitativo y Cuantitativo'!C47</f>
         <v>R15</v>
       </c>
-      <c r="E22" s="146">
+      <c r="E22" s="154">
         <f>'Cualitativo y Cuantitativo'!D47</f>
         <v>0</v>
       </c>
-      <c r="F22" s="146"/>
+      <c r="F22" s="154"/>
       <c r="G22" s="81" t="str">
         <f>'Cualitativo y Cuantitativo'!F47</f>
         <v>MUY BAJO</v>
@@ -4767,8 +4978,8 @@
         <f>'Cualitativo y Cuantitativo'!J47</f>
         <v>0</v>
       </c>
-      <c r="M22" s="146"/>
-      <c r="N22" s="146"/>
+      <c r="M22" s="154"/>
+      <c r="N22" s="154"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
@@ -4818,6 +5029,29 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C5:O5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E22:F22"/>
@@ -4828,29 +5062,6 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C5:O5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="M8:N8"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4877,8 +5088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4892,7 +5103,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="147" t="s">
+      <c r="B5" s="157" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="83">
@@ -4925,7 +5136,7 @@
       <c r="N5" s="84"/>
     </row>
     <row r="6" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="147"/>
+      <c r="B6" s="157"/>
       <c r="C6" s="83">
         <v>4</v>
       </c>
@@ -4956,7 +5167,7 @@
       <c r="N6" s="84"/>
     </row>
     <row r="7" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="147"/>
+      <c r="B7" s="157"/>
       <c r="C7" s="83">
         <v>3</v>
       </c>
@@ -4974,11 +5185,11 @@
       </c>
       <c r="G7" s="114" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=4)," R15"," "))</f>
-        <v xml:space="preserve"> R2             </v>
+        <v xml:space="preserve">R1R2R3 R5          </v>
       </c>
       <c r="H7" s="115" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=3,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=3,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=3,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=3,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=3,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=3,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=3,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=3,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=3,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=3,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=3,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=3,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=3,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=3,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=3,Matriz!I29=5)," R15"," "))</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">     R6         </v>
       </c>
       <c r="J7" s="84"/>
       <c r="K7" s="84"/>
@@ -4987,7 +5198,7 @@
       <c r="N7" s="84"/>
     </row>
     <row r="8" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="147"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="83">
         <v>2</v>
       </c>
@@ -5001,11 +5212,11 @@
       </c>
       <c r="F8" s="114" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=3),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=3),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=3),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=3),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=3),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=3),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=3)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=3)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=3)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=3)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=3)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=3)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=3)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=3)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=3)," R15"," "))</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">   R4           </v>
       </c>
       <c r="G8" s="114" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=4),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=4),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=4),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=4),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=4),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=4),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=4)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=4)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=4)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=4)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=4)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=4)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=4)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=4)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=4)," R15"," "))</f>
-        <v xml:space="preserve">R1              </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="H8" s="115" t="str">
         <f>CONCATENATE(  IF(AND(Matriz!H16=2,Matriz!I16=5),"R1", " "), IF(AND(Matriz!H17=2,Matriz!I17=5),"R2", " "), IF(AND(Matriz!H18=2,Matriz!I18=5),"R3", " "), IF(AND(Matriz!H19=2,Matriz!I19=5),"R4", " "), IF(AND(Matriz!H20=2,Matriz!I20=5),"R5", " "), IF(AND(Matriz!H21=2,Matriz!I21=5),"R6", " "),IF(AND(Matriz!H22=2,Matriz!I22=5)," R7"," "),IF(AND(Matriz!H23=2,Matriz!I23=5)," R8"," "),IF(AND(Matriz!H24=2,Matriz!I24=5)," R9"," "),IF(AND(Matriz!H25=2,Matriz!I25=5)," R10"," "),IF(AND(Matriz!H26=2,Matriz!I26=5)," R11"," "),IF(AND(Matriz!H27=2,Matriz!I27=5)," R12"," "),IF(AND(Matriz!H28=2,Matriz!I28=5)," R13"," "),IF(AND(Matriz!H28=2,Matriz!I28=5)," R14"," "),IF(AND(Matriz!H29=2,Matriz!I29=5)," R15"," "))</f>
@@ -5018,7 +5229,7 @@
       <c r="N8" s="84"/>
     </row>
     <row r="9" spans="2:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="147"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="83">
         <v>1</v>
       </c>
@@ -5067,13 +5278,13 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="148" t="s">
+      <c r="D11" s="158" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="148"/>
-      <c r="F11" s="148"/>
-      <c r="G11" s="148"/>
-      <c r="H11" s="148"/>
+      <c r="E11" s="158"/>
+      <c r="F11" s="158"/>
+      <c r="G11" s="158"/>
+      <c r="H11" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5094,7 +5305,7 @@
   <dimension ref="D6:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5103,10 +5314,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="149" t="s">
+      <c r="D6" s="159" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="149"/>
+      <c r="E6" s="159"/>
       <c r="G6" t="s">
         <v>64</v>
       </c>

</xml_diff>